<commit_message>
Name des Datenblattes geändert
Artikelpreisliste Namenänderung im Datenblatt
</commit_message>
<xml_diff>
--- a/data/Artikelpreisliste.xlsx
+++ b/data/Artikelpreisliste.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/563ce15318b10045/GitHub-Projekte/haas-preisliste-viewer/haas-preisliste-viewer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{C16FD66B-CDD3-46C6-925A-7F8351258248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2915456E-59DA-4E08-B46F-1C1CB7588EB7}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{C16FD66B-CDD3-46C6-925A-7F8351258248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14765D91-519F-4D28-8DBC-FAC3DBBC4908}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15120" tabRatio="842" xr2:uid="{E306DA56-BA47-4E63-9DB7-853595B00539}"/>
   </bookViews>
   <sheets>
-    <sheet name="Artikelpreisliste_11-2025" sheetId="10" r:id="rId1"/>
+    <sheet name="Artikelpreisliste_11-2025(V)" sheetId="10" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Artikelpreisliste_11-2025'!$A$1:$G$850</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Artikelpreisliste_11-2025'!$A$1:$G$850</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Artikelpreisliste_11-2025(V)'!$A$1:$G$850</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Artikelpreisliste_11-2025(V)'!$A$1:$G$850</definedName>
     <definedName name="Überschrift" localSheetId="0">[1]Seite1_Druckversion!#REF!</definedName>
     <definedName name="Überschrift">#REF!</definedName>
   </definedNames>
@@ -9263,6 +9263,10 @@
 </externalLink>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
@@ -27610,6 +27614,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="ab8bd484-5ca4-4a73-9d13-e00aa543dd09">
@@ -27618,15 +27631,6 @@
     <TaxCatchAll xmlns="6409ede6-a842-48c9-9732-19d8afc3fd29" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -27649,6 +27653,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70291D3E-9502-4216-AA50-1FFA8B03D83A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC974967-B322-408C-935B-E6A1CB4FB0BD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -27657,12 +27669,4 @@
     <ds:schemaRef ds:uri="6409ede6-a842-48c9-9732-19d8afc3fd29"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70291D3E-9502-4216-AA50-1FFA8B03D83A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>